<commit_message>
Script para adicionar novas pessoas a cena
</commit_message>
<xml_diff>
--- a/Assets/DadosExternos/DadosDaRotina.xlsx
+++ b/Assets/DadosExternos/DadosDaRotina.xlsx
@@ -13,10 +13,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1603819537" val="978" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1603819537" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1603819537" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1603819537"/>
+      <pm:revision xmlns:pm="smNativeData" day="1607205190" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1607205190" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1607205190" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1607205190"/>
     </ext>
   </extLst>
 </workbook>
@@ -83,7 +83,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1603819537" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1607205190" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -105,7 +105,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1603819537" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1607205190" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -127,7 +127,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1603819537"/>
+          <pm:border xmlns:pm="smNativeData" id="1607205190"/>
         </ext>
       </extLst>
     </border>
@@ -146,7 +146,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1603819537"/>
+          <pm:border xmlns:pm="smNativeData" id="1607205190"/>
         </ext>
       </extLst>
     </border>
@@ -163,7 +163,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1603819537" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1607205190" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -427,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -563,11 +563,87 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>28</v>
+      </c>
+      <c r="G4" t="n">
+        <v>13</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>23</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>10</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>13</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>12</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>22</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>9</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1603819537" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1607205190" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -576,14 +652,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1603819537" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1603819537" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1607205190" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1607205190" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1603819537" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1607205190" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>